<commit_message>
Added check for valid frequency!
</commit_message>
<xml_diff>
--- a/BAYRFGW17_LSM_EMPLOYEE_Channels_sessions.xlsx
+++ b/BAYRFGW17_LSM_EMPLOYEE_Channels_sessions.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scascio/GitHub/LSM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sacascio/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="46280" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BAYRFGW17_LSM_EMPLOYEE_Channels" sheetId="1" r:id="rId1"/>
@@ -380,7 +380,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>